<commit_message>
switch ON the "L1_DoubleMu18er2p1_SQ" seed
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-13.6TeV_RampUp.xlsx
+++ b/official/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-13.6TeV_RampUp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_2_0_off/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF56550-6F0E-EF4E-B3FB-84CB62F1BFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D276AF-0CC5-844B-82FA-8DCB5FE7781B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1714,10 +1714,10 @@
   <dimension ref="A1:AN1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7688,13 +7688,13 @@
         <v>0</v>
       </c>
       <c r="N50" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P50" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="11">
         <v>0</v>
@@ -56346,17 +56346,17 @@
       <c r="M1010" s="20"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AH599 AI3:AN398">
+  <conditionalFormatting sqref="AI3:AN398 C3:AH599">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:AH599 AI3:AN398">
+  <conditionalFormatting sqref="AI3:AN398 C3:AH599">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:AH599 AI3:AN398">
+  <conditionalFormatting sqref="AI3:AN398 C3:AH599">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>